<commit_message>
added stats for v4..
</commit_message>
<xml_diff>
--- a/preprocessing/Model_Stats.xlsx
+++ b/preprocessing/Model_Stats.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Desktop\project-piscator\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69158212-F27C-4294-A8EF-9FBEE5F7948E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F260F1-4944-4C0F-A938-69BA38E47928}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
   </bookViews>
   <sheets>
-    <sheet name="PhishingForestV2" sheetId="1" r:id="rId1"/>
-    <sheet name="PhishingForestV2 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="V2" sheetId="1" r:id="rId1"/>
+    <sheet name="V3" sheetId="2" r:id="rId2"/>
+    <sheet name="V4" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
   <si>
     <t>Jonathan_Mailbox</t>
   </si>
@@ -140,6 +141,15 @@
   </si>
   <si>
     <t>disregard olden day data - current model only trained with modern day data. With a super small sample and test size of modern day phish it seems fairly accurate, and no ham have been identified wrongly so far. Probably need more data to test</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>dsv4.csv</t>
+  </si>
+  <si>
+    <t>model test of sample size 15 after implementing mx, dkim, spf, dmarc. Fairly inaccurate… only detects 50% on average, we probably need more phishing emails</t>
   </si>
 </sst>
 </file>
@@ -255,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -282,11 +292,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="72">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -388,6 +400,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -397,6 +425,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -406,6 +450,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -415,6 +475,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -440,6 +516,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -456,6 +541,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -472,6 +566,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -485,6 +585,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -506,13 +618,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="27" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="44">
+    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="66">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -520,14 +632,59 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="26" dataDxfId="42">
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A3F97E-A535-4D7B-8BA9-370DCCBB0340}" name="Table46123" displayName="Table46123" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{275D5550-6ADB-43C4-BF7E-D2168244788F}" name="S/N" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{AD3A6138-B32C-4A9C-9861-0910BA8C7CF0}" name="Detection Count" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{53AB10D9-475E-498A-A010-18523684D9F0}" name="Sample Size" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{CCFFD2CF-6724-4423-818F-6CFEEFBF3A0E}" name="Accuracy" dataDxfId="12">
+      <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B875B3D-C2EE-4CFF-BC4C-4BF1588E5042}" name="Table49134" displayName="Table49134" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E920ABA6-44F5-4C28-8A5E-0C0A6482E954}" name="S/N" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0C7661B2-A4AD-4B35-8F73-6ED9583A18F9}" name="Detection Count" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{77DE6E9C-DB96-403B-9A7A-3CD37F43427E}" name="Sample Size" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{81917785-C766-46C0-A868-C83148F4C68F}" name="Accuracy" dataDxfId="6">
+      <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2D337A66-8B74-438F-A66D-6DAE14683A0E}" name="Table4610147" displayName="Table4610147" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E34AB060-FD1F-4F17-B6E3-FCB710023011}" name="S/N" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{7E19895C-182A-4984-AA78-7637705A8A27}" name="Detection Count" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{6D3C562D-AD07-4C05-820F-DBF3059539B1}" name="Sample Size" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A053C10B-B044-4B72-912A-420CCD660884}" name="Accuracy" dataDxfId="0">
+      <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+  <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="60">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -536,13 +693,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="24" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="54">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -551,13 +708,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="25" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="48">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -566,13 +723,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="42">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -581,13 +738,13 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="36">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -596,13 +753,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="30">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -611,14 +768,29 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="24">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8836F220-A1C5-4260-B70B-3506874B3BA5}" name="Table4112" displayName="Table4112" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B75D1CA6-6206-4228-BDCB-E56D23E710CF}" name="S/N" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{E0B715E6-3A0A-4312-B101-82F14F11CFBF}" name="Detection Count" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{72DD18F7-2B09-4F23-ADF4-C0C79EC302A9}" name="Sample Size" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{C140A7CC-F574-4E1F-8F2C-BD831A012684}" name="Accuracy" dataDxfId="18">
+      <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -925,7 +1097,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B4" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E4A342-217B-46FA-804C-B78B10A22114}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -2012,4 +2184,540 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264BC4D7-18E1-4FBD-B4C5-EC64A6B4AF4A}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>694</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>425</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>132</v>
+      </c>
+      <c r="F4" s="10">
+        <v>132</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G8" si="0">(E4/F4)*100</f>
+        <v>100</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>296</v>
+      </c>
+      <c r="K4" s="10">
+        <v>299</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ref="L4:L8" si="1">(J4/K4)*100</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>132</v>
+      </c>
+      <c r="F5" s="10">
+        <v>132</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>296</v>
+      </c>
+      <c r="K5" s="10">
+        <v>299</v>
+      </c>
+      <c r="L5" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10">
+        <v>132</v>
+      </c>
+      <c r="F6" s="10">
+        <v>132</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" s="10">
+        <v>296</v>
+      </c>
+      <c r="K6" s="10">
+        <v>299</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10">
+        <v>132</v>
+      </c>
+      <c r="F7" s="10">
+        <v>132</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10">
+        <v>296</v>
+      </c>
+      <c r="K7" s="10">
+        <v>299</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUM(B2:B6)</f>
+        <v>1119</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>132</v>
+      </c>
+      <c r="F8" s="10">
+        <v>132</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+      <c r="J8" s="10">
+        <v>296</v>
+      </c>
+      <c r="K8" s="10">
+        <v>299</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8">
+        <f>AVERAGE(G4:G8)</f>
+        <v>100</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="8">
+        <f>AVERAGE(L4:L8)</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="D12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="D13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>6</v>
+      </c>
+      <c r="F14" s="10">
+        <v>15</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" ref="G14:G18" si="2">(E14/F14)*100</f>
+        <v>40</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
+        <v>32</v>
+      </c>
+      <c r="K14" s="10">
+        <v>299</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" ref="L14:L18" si="3">(J14/K14)*100</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>8</v>
+      </c>
+      <c r="F15" s="10">
+        <v>15</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="2"/>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="I15" s="10">
+        <v>2</v>
+      </c>
+      <c r="J15" s="10">
+        <v>32</v>
+      </c>
+      <c r="K15" s="10">
+        <v>299</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUM(B11:B14)</f>
+        <v>30</v>
+      </c>
+      <c r="D16" s="10">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>8</v>
+      </c>
+      <c r="F16" s="10">
+        <v>15</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="2"/>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="I16" s="10">
+        <v>3</v>
+      </c>
+      <c r="J16" s="10">
+        <v>32</v>
+      </c>
+      <c r="K16" s="10">
+        <v>299</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="10">
+        <v>4</v>
+      </c>
+      <c r="E17" s="10">
+        <v>7</v>
+      </c>
+      <c r="F17" s="10">
+        <v>15</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="2"/>
+        <v>46.666666666666664</v>
+      </c>
+      <c r="I17" s="10">
+        <v>4</v>
+      </c>
+      <c r="J17" s="10">
+        <v>32</v>
+      </c>
+      <c r="K17" s="10">
+        <v>299</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B8+B16</f>
+        <v>1149</v>
+      </c>
+      <c r="D18" s="10">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>9</v>
+      </c>
+      <c r="F18" s="10">
+        <v>15</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="I18" s="10">
+        <v>5</v>
+      </c>
+      <c r="J18" s="10">
+        <v>32</v>
+      </c>
+      <c r="K18" s="10">
+        <v>299</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="8">
+        <f>AVERAGE(G14:G18)</f>
+        <v>50.666666666666671</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="8">
+        <f>AVERAGE(L14:L18)</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13">
+        <f>AVERAGE(G10+G20)/2</f>
+        <v>75.333333333333343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
version 6 model, Ds updated with 3 new labels
</commit_message>
<xml_diff>
--- a/preprocessing/Model_Stats.xlsx
+++ b/preprocessing/Model_Stats.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Desktop\project-piscator\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4848328B-B5B9-4251-AFDA-715F8F416955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBAC028-9149-44AA-8DD8-DA8E2BDBD739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
   </bookViews>
   <sheets>
     <sheet name="V2" sheetId="1" r:id="rId1"/>
     <sheet name="V3" sheetId="2" r:id="rId2"/>
     <sheet name="V4" sheetId="3" r:id="rId3"/>
     <sheet name="V5" sheetId="4" r:id="rId4"/>
+    <sheet name="V6" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="46">
   <si>
     <t>Jonathan_Mailbox</t>
   </si>
@@ -166,6 +167,15 @@
   </si>
   <si>
     <t>Retrained model with new data on modern phish, accuracy improved to 75.6% on 5 runs. N_estimators=100 worked OK.</t>
+  </si>
+  <si>
+    <t>dsv5.csv</t>
+  </si>
+  <si>
+    <t>dsv6.csv</t>
+  </si>
+  <si>
+    <t>Retrained model with 3 new additional labels. Generally same accuracy with slight increase. Some emails unable to parse the 3 new labels, probably because get_content returned null so score was 0</t>
   </si>
 </sst>
 </file>
@@ -314,7 +324,107 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="120">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -734,13 +844,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="90">
+    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="114">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -749,13 +859,13 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A3F97E-A535-4D7B-8BA9-370DCCBB0340}" name="Table46123" displayName="Table46123" ref="D13:G18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A3F97E-A535-4D7B-8BA9-370DCCBB0340}" name="Table46123" displayName="Table46123" ref="D13:G18" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{275D5550-6ADB-43C4-BF7E-D2168244788F}" name="S/N" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{AD3A6138-B32C-4A9C-9861-0910BA8C7CF0}" name="Detection Count" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{53AB10D9-475E-498A-A010-18523684D9F0}" name="Sample Size" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{CCFFD2CF-6724-4423-818F-6CFEEFBF3A0E}" name="Accuracy" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{275D5550-6ADB-43C4-BF7E-D2168244788F}" name="S/N" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{AD3A6138-B32C-4A9C-9861-0910BA8C7CF0}" name="Detection Count" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{53AB10D9-475E-498A-A010-18523684D9F0}" name="Sample Size" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{CCFFD2CF-6724-4423-818F-6CFEEFBF3A0E}" name="Accuracy" dataDxfId="60">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -764,13 +874,13 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B875B3D-C2EE-4CFF-BC4C-4BF1588E5042}" name="Table49134" displayName="Table49134" ref="I3:L8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B875B3D-C2EE-4CFF-BC4C-4BF1588E5042}" name="Table49134" displayName="Table49134" ref="I3:L8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E920ABA6-44F5-4C28-8A5E-0C0A6482E954}" name="S/N" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{0C7661B2-A4AD-4B35-8F73-6ED9583A18F9}" name="Detection Count" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{77DE6E9C-DB96-403B-9A7A-3CD37F43427E}" name="Sample Size" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{81917785-C766-46C0-A868-C83148F4C68F}" name="Accuracy" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{E920ABA6-44F5-4C28-8A5E-0C0A6482E954}" name="S/N" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{0C7661B2-A4AD-4B35-8F73-6ED9583A18F9}" name="Detection Count" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{77DE6E9C-DB96-403B-9A7A-3CD37F43427E}" name="Sample Size" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{81917785-C766-46C0-A868-C83148F4C68F}" name="Accuracy" dataDxfId="54">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -779,13 +889,13 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2D337A66-8B74-438F-A66D-6DAE14683A0E}" name="Table4610147" displayName="Table4610147" ref="I13:L18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2D337A66-8B74-438F-A66D-6DAE14683A0E}" name="Table4610147" displayName="Table4610147" ref="I13:L18" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E34AB060-FD1F-4F17-B6E3-FCB710023011}" name="S/N" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{7E19895C-182A-4984-AA78-7637705A8A27}" name="Detection Count" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{6D3C562D-AD07-4C05-820F-DBF3059539B1}" name="Sample Size" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{A053C10B-B044-4B72-912A-420CCD660884}" name="Accuracy" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{E34AB060-FD1F-4F17-B6E3-FCB710023011}" name="S/N" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{7E19895C-182A-4984-AA78-7637705A8A27}" name="Detection Count" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{6D3C562D-AD07-4C05-820F-DBF3059539B1}" name="Sample Size" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{A053C10B-B044-4B72-912A-420CCD660884}" name="Accuracy" dataDxfId="48">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -794,13 +904,13 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15DF06F2-BFC5-400B-8F8E-C4A82BD5CA00}" name="Table41128" displayName="Table41128" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15DF06F2-BFC5-400B-8F8E-C4A82BD5CA00}" name="Table41128" displayName="Table41128" ref="D3:G8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C753AC17-EEBF-4341-A85D-76065FABCBE7}" name="S/N" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{245102FA-69F1-4066-AF28-CCDAAA350CB3}" name="Detection Count" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{92689FC9-DDA3-4F25-8EFE-6CC23F93898B}" name="Sample Size" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{85C2FEF5-4AE8-4949-8ED0-C79CFBE661FB}" name="Accuracy" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{C753AC17-EEBF-4341-A85D-76065FABCBE7}" name="S/N" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{245102FA-69F1-4066-AF28-CCDAAA350CB3}" name="Detection Count" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{92689FC9-DDA3-4F25-8EFE-6CC23F93898B}" name="Sample Size" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{85C2FEF5-4AE8-4949-8ED0-C79CFBE661FB}" name="Accuracy" dataDxfId="42">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -809,13 +919,13 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B5E58A1E-73FE-4AB3-B879-E930B517F804}" name="Table4612315" displayName="Table4612315" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B5E58A1E-73FE-4AB3-B879-E930B517F804}" name="Table4612315" displayName="Table4612315" ref="D13:G18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{61A9D479-03E6-4200-94BF-A8DDEA70FEBF}" name="S/N" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{6050BD2E-D7F1-4053-A601-F41A8D89209F}" name="Detection Count" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{DD2DA752-841B-4E27-9369-82F77478078E}" name="Sample Size" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{64DD8FB3-6B62-43F6-89C0-49A140C3CF49}" name="Accuracy" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{61A9D479-03E6-4200-94BF-A8DDEA70FEBF}" name="S/N" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{6050BD2E-D7F1-4053-A601-F41A8D89209F}" name="Detection Count" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{DD2DA752-841B-4E27-9369-82F77478078E}" name="Sample Size" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{64DD8FB3-6B62-43F6-89C0-49A140C3CF49}" name="Accuracy" dataDxfId="36">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -824,13 +934,13 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BCD2CAA6-E938-457D-BB91-89990D3D2810}" name="Table4913416" displayName="Table4913416" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BCD2CAA6-E938-457D-BB91-89990D3D2810}" name="Table4913416" displayName="Table4913416" ref="I3:L8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C991C267-3048-4225-B828-12E25D3E5025}" name="S/N" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{762A4A20-DDB2-474A-8744-7CECF83980B1}" name="Detection Count" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{08F95622-5A81-4212-AE47-92A0246F77EC}" name="Sample Size" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{52BB0AE4-B04C-4A77-962C-287EC8E5F665}" name="Accuracy" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{C991C267-3048-4225-B828-12E25D3E5025}" name="S/N" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{762A4A20-DDB2-474A-8744-7CECF83980B1}" name="Detection Count" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{08F95622-5A81-4212-AE47-92A0246F77EC}" name="Sample Size" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{52BB0AE4-B04C-4A77-962C-287EC8E5F665}" name="Accuracy" dataDxfId="30">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -839,13 +949,13 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CB6C8DE4-CA53-4725-B7F8-AA492457AAE7}" name="Table461014717" displayName="Table461014717" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CB6C8DE4-CA53-4725-B7F8-AA492457AAE7}" name="Table461014717" displayName="Table461014717" ref="I13:L18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9C4BC6FC-1B17-4A97-96D3-43004D220CAE}" name="S/N" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{15BE8F3E-E6BD-4F8A-A09A-BC176454914E}" name="Detection Count" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A567ED6E-D3B6-4394-AF09-84C5732DC7B7}" name="Sample Size" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{5C74BD57-2650-4F27-A620-D6FE482814D1}" name="Accuracy" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{9C4BC6FC-1B17-4A97-96D3-43004D220CAE}" name="S/N" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{15BE8F3E-E6BD-4F8A-A09A-BC176454914E}" name="Detection Count" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{A567ED6E-D3B6-4394-AF09-84C5732DC7B7}" name="Sample Size" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{5C74BD57-2650-4F27-A620-D6FE482814D1}" name="Accuracy" dataDxfId="24">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -853,14 +963,29 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{32A616EB-A77D-4F38-AEF8-2444FD4EF958}" name="Table4112818" displayName="Table4112818" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{2465D8E4-C5BF-4E81-AAEA-6B1E212E7BBD}" name="S/N" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{F0DD74ED-14AB-4A12-8DC6-7E49A5ACD8AC}" name="Detection Count" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0681E460-8849-486E-8A3F-22055197C330}" name="Sample Size" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{6457E6E5-B2B0-4B8E-B3FB-47649ACD14D0}" name="Accuracy" dataDxfId="18">
+      <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{9CC61B1E-103F-4412-872D-2E234673F946}" name="Table461231519" displayName="Table461231519" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="84">
+    <tableColumn id="1" xr3:uid="{9F38C2E0-46F3-41C3-A5E6-EEEE64A2589F}" name="S/N" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{35F01D39-81DD-4978-AF87-26C70E04D654}" name="Detection Count" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{4744942B-C705-4E3F-A247-958A2EB2E913}" name="Sample Size" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{BBE1D400-C4DA-4403-BE90-442D8886004B}" name="Accuracy" dataDxfId="12">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -868,14 +993,59 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{589BC326-89DF-42FE-ADBB-E4FF113CEBDB}" name="Table491341620" displayName="Table491341620" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{CCE9E2BE-0E17-41BE-967B-EE16AA992DDB}" name="S/N" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{A7484308-39BA-4A28-9275-04DDFE2DFFEB}" name="Detection Count" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{2C4DCCF1-C4C2-4E4E-8BAF-B54EC7908178}" name="Sample Size" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{22839C3C-360C-4234-AFB5-FBBD81DFB55B}" name="Accuracy" dataDxfId="6">
+      <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+  <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="108">
+      <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{6A0B21C2-72D0-4357-9836-2DED7539C21E}" name="Table46101471721" displayName="Table46101471721" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3258CFBC-6680-43C6-9D44-B8C132BDFF7E}" name="S/N" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{0C464FE1-A4AA-4ED8-8F75-83194D25D87B}" name="Detection Count" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1977B50C-B9C1-44F2-BFF0-2D4C47585C51}" name="Sample Size" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BA3CF17C-3E2E-4212-BDE3-20DA51952E02}" name="Accuracy" dataDxfId="0">
+      <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+  <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="102">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -884,13 +1054,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="96">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -899,13 +1069,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="66">
+    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="90">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -914,13 +1084,13 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="84">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -929,13 +1099,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="78">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -944,13 +1114,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="72">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -959,13 +1129,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8836F220-A1C5-4260-B70B-3506874B3BA5}" name="Table4112" displayName="Table4112" ref="D3:G8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8836F220-A1C5-4260-B70B-3506874B3BA5}" name="Table4112" displayName="Table4112" ref="D3:G8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B75D1CA6-6206-4228-BDCB-E56D23E710CF}" name="S/N" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{E0B715E6-3A0A-4312-B101-82F14F11CFBF}" name="Detection Count" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{72DD18F7-2B09-4F23-ADF4-C0C79EC302A9}" name="Sample Size" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{C140A7CC-F574-4E1F-8F2C-BD831A012684}" name="Accuracy" dataDxfId="42">
+    <tableColumn id="1" xr3:uid="{B75D1CA6-6206-4228-BDCB-E56D23E710CF}" name="S/N" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{E0B715E6-3A0A-4312-B101-82F14F11CFBF}" name="Detection Count" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{72DD18F7-2B09-4F23-ADF4-C0C79EC302A9}" name="Sample Size" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{C140A7CC-F574-4E1F-8F2C-BD831A012684}" name="Accuracy" dataDxfId="66">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2902,8 +3072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4DBE0C-94A2-4F25-B84B-83E2584B0B86}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3405,7 +3575,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
@@ -3432,6 +3602,554 @@
     <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACAC222-742D-4DC0-B4CC-329DB85D9DEF}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>694</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>425</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2">
+        <v>332</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>133</v>
+      </c>
+      <c r="F4" s="10">
+        <v>134</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G8" si="0">(E4/F4)*100</f>
+        <v>99.253731343283576</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>296</v>
+      </c>
+      <c r="K4" s="10">
+        <v>299</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ref="L4:L8" si="1">(J4/K4)*100</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>134</v>
+      </c>
+      <c r="F5" s="10">
+        <v>134</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>296</v>
+      </c>
+      <c r="K5" s="10">
+        <v>299</v>
+      </c>
+      <c r="L5" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10">
+        <v>133</v>
+      </c>
+      <c r="F6" s="10">
+        <v>134</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>99.253731343283576</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" s="10">
+        <v>296</v>
+      </c>
+      <c r="K6" s="10">
+        <v>299</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10">
+        <v>133</v>
+      </c>
+      <c r="F7" s="10">
+        <v>134</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>99.253731343283576</v>
+      </c>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10">
+        <v>296</v>
+      </c>
+      <c r="K7" s="10">
+        <v>299</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUM(B2:B6)</f>
+        <v>1451</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>133</v>
+      </c>
+      <c r="F8" s="10">
+        <v>134</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.253731343283576</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+      <c r="J8" s="10">
+        <v>296</v>
+      </c>
+      <c r="K8" s="10">
+        <v>299</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8">
+        <f>AVERAGE(G4:G8)</f>
+        <v>99.402985074626855</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="8">
+        <f>AVERAGE(L4:L8)</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3">
+        <v>81</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3">
+        <v>15</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>31</v>
+      </c>
+      <c r="F14" s="10">
+        <v>41</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" ref="G14:G18" si="2">(E14/F14)*100</f>
+        <v>75.609756097560975</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
+        <v>32</v>
+      </c>
+      <c r="K14" s="10">
+        <v>299</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" ref="L14:L18" si="3">(J14/K14)*100</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>32</v>
+      </c>
+      <c r="F15" s="10">
+        <v>41</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="2"/>
+        <v>78.048780487804876</v>
+      </c>
+      <c r="I15" s="10">
+        <v>2</v>
+      </c>
+      <c r="J15" s="10">
+        <v>32</v>
+      </c>
+      <c r="K15" s="10">
+        <v>299</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUM(B11:B14)</f>
+        <v>141</v>
+      </c>
+      <c r="D16" s="10">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>30</v>
+      </c>
+      <c r="F16" s="10">
+        <v>41</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="2"/>
+        <v>73.170731707317074</v>
+      </c>
+      <c r="I16" s="10">
+        <v>3</v>
+      </c>
+      <c r="J16" s="10">
+        <v>32</v>
+      </c>
+      <c r="K16" s="10">
+        <v>299</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="10">
+        <v>4</v>
+      </c>
+      <c r="E17" s="10">
+        <v>31</v>
+      </c>
+      <c r="F17" s="10">
+        <v>41</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="2"/>
+        <v>75.609756097560975</v>
+      </c>
+      <c r="I17" s="10">
+        <v>4</v>
+      </c>
+      <c r="J17" s="10">
+        <v>32</v>
+      </c>
+      <c r="K17" s="10">
+        <v>299</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B8+B16</f>
+        <v>1592</v>
+      </c>
+      <c r="D18" s="10">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>32</v>
+      </c>
+      <c r="F18" s="10">
+        <v>41</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="2"/>
+        <v>78.048780487804876</v>
+      </c>
+      <c r="I18" s="10">
+        <v>5</v>
+      </c>
+      <c r="J18" s="10">
+        <v>32</v>
+      </c>
+      <c r="K18" s="10">
+        <v>299</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="8">
+        <f>AVERAGE(G14:G18)</f>
+        <v>76.097560975609753</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="8">
+        <f>AVERAGE(L14:L18)</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13">
+        <f>AVERAGE(G10+G20)/2</f>
+        <v>87.750273025118304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
serialized version 7 of model with more data. 79% phishing, 89% accuracy overall
</commit_message>
<xml_diff>
--- a/preprocessing/Model_Stats.xlsx
+++ b/preprocessing/Model_Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Desktop\project-piscator\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBAC028-9149-44AA-8DD8-DA8E2BDBD739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E052E0-AAD0-4969-9DED-093723B42DF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
   </bookViews>
   <sheets>
     <sheet name="V2" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="V4" sheetId="3" r:id="rId3"/>
     <sheet name="V5" sheetId="4" r:id="rId4"/>
     <sheet name="V6" sheetId="5" r:id="rId5"/>
+    <sheet name="V7" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="51">
   <si>
     <t>Jonathan_Mailbox</t>
   </si>
@@ -176,6 +177,21 @@
   </si>
   <si>
     <t>Retrained model with 3 new additional labels. Generally same accuracy with slight increase. Some emails unable to parse the 3 new labels, probably because get_content returned null so score was 0</t>
+  </si>
+  <si>
+    <t>Yannis_Mailbox</t>
+  </si>
+  <si>
+    <t>ModernHam1</t>
+  </si>
+  <si>
+    <t>ModernPhish2</t>
+  </si>
+  <si>
+    <t>dsv7.csv</t>
+  </si>
+  <si>
+    <t>Added about 40 mote items to train and increased phishing sample size. Model sits at about 79.6% right now, conclusion: requires more phishing emails</t>
   </si>
 </sst>
 </file>
@@ -324,7 +340,107 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="144">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -844,13 +960,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="116"/>
-    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="114">
+    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="138">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -859,13 +975,13 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A3F97E-A535-4D7B-8BA9-370DCCBB0340}" name="Table46123" displayName="Table46123" ref="D13:G18" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A3F97E-A535-4D7B-8BA9-370DCCBB0340}" name="Table46123" displayName="Table46123" ref="D13:G18" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{275D5550-6ADB-43C4-BF7E-D2168244788F}" name="S/N" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{AD3A6138-B32C-4A9C-9861-0910BA8C7CF0}" name="Detection Count" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{53AB10D9-475E-498A-A010-18523684D9F0}" name="Sample Size" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{CCFFD2CF-6724-4423-818F-6CFEEFBF3A0E}" name="Accuracy" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{275D5550-6ADB-43C4-BF7E-D2168244788F}" name="S/N" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{AD3A6138-B32C-4A9C-9861-0910BA8C7CF0}" name="Detection Count" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{53AB10D9-475E-498A-A010-18523684D9F0}" name="Sample Size" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{CCFFD2CF-6724-4423-818F-6CFEEFBF3A0E}" name="Accuracy" dataDxfId="84">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -874,13 +990,13 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B875B3D-C2EE-4CFF-BC4C-4BF1588E5042}" name="Table49134" displayName="Table49134" ref="I3:L8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B875B3D-C2EE-4CFF-BC4C-4BF1588E5042}" name="Table49134" displayName="Table49134" ref="I3:L8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E920ABA6-44F5-4C28-8A5E-0C0A6482E954}" name="S/N" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{0C7661B2-A4AD-4B35-8F73-6ED9583A18F9}" name="Detection Count" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{77DE6E9C-DB96-403B-9A7A-3CD37F43427E}" name="Sample Size" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{81917785-C766-46C0-A868-C83148F4C68F}" name="Accuracy" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{E920ABA6-44F5-4C28-8A5E-0C0A6482E954}" name="S/N" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{0C7661B2-A4AD-4B35-8F73-6ED9583A18F9}" name="Detection Count" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{77DE6E9C-DB96-403B-9A7A-3CD37F43427E}" name="Sample Size" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{81917785-C766-46C0-A868-C83148F4C68F}" name="Accuracy" dataDxfId="78">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -889,13 +1005,13 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2D337A66-8B74-438F-A66D-6DAE14683A0E}" name="Table4610147" displayName="Table4610147" ref="I13:L18" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2D337A66-8B74-438F-A66D-6DAE14683A0E}" name="Table4610147" displayName="Table4610147" ref="I13:L18" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E34AB060-FD1F-4F17-B6E3-FCB710023011}" name="S/N" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{7E19895C-182A-4984-AA78-7637705A8A27}" name="Detection Count" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{6D3C562D-AD07-4C05-820F-DBF3059539B1}" name="Sample Size" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{A053C10B-B044-4B72-912A-420CCD660884}" name="Accuracy" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{E34AB060-FD1F-4F17-B6E3-FCB710023011}" name="S/N" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{7E19895C-182A-4984-AA78-7637705A8A27}" name="Detection Count" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{6D3C562D-AD07-4C05-820F-DBF3059539B1}" name="Sample Size" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{A053C10B-B044-4B72-912A-420CCD660884}" name="Accuracy" dataDxfId="72">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -904,13 +1020,13 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15DF06F2-BFC5-400B-8F8E-C4A82BD5CA00}" name="Table41128" displayName="Table41128" ref="D3:G8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15DF06F2-BFC5-400B-8F8E-C4A82BD5CA00}" name="Table41128" displayName="Table41128" ref="D3:G8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C753AC17-EEBF-4341-A85D-76065FABCBE7}" name="S/N" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{245102FA-69F1-4066-AF28-CCDAAA350CB3}" name="Detection Count" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{92689FC9-DDA3-4F25-8EFE-6CC23F93898B}" name="Sample Size" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{85C2FEF5-4AE8-4949-8ED0-C79CFBE661FB}" name="Accuracy" dataDxfId="42">
+    <tableColumn id="1" xr3:uid="{C753AC17-EEBF-4341-A85D-76065FABCBE7}" name="S/N" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{245102FA-69F1-4066-AF28-CCDAAA350CB3}" name="Detection Count" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{92689FC9-DDA3-4F25-8EFE-6CC23F93898B}" name="Sample Size" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{85C2FEF5-4AE8-4949-8ED0-C79CFBE661FB}" name="Accuracy" dataDxfId="66">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -919,13 +1035,13 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B5E58A1E-73FE-4AB3-B879-E930B517F804}" name="Table4612315" displayName="Table4612315" ref="D13:G18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B5E58A1E-73FE-4AB3-B879-E930B517F804}" name="Table4612315" displayName="Table4612315" ref="D13:G18" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{61A9D479-03E6-4200-94BF-A8DDEA70FEBF}" name="S/N" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{6050BD2E-D7F1-4053-A601-F41A8D89209F}" name="Detection Count" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{DD2DA752-841B-4E27-9369-82F77478078E}" name="Sample Size" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{64DD8FB3-6B62-43F6-89C0-49A140C3CF49}" name="Accuracy" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{61A9D479-03E6-4200-94BF-A8DDEA70FEBF}" name="S/N" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{6050BD2E-D7F1-4053-A601-F41A8D89209F}" name="Detection Count" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{DD2DA752-841B-4E27-9369-82F77478078E}" name="Sample Size" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{64DD8FB3-6B62-43F6-89C0-49A140C3CF49}" name="Accuracy" dataDxfId="60">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -934,13 +1050,13 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BCD2CAA6-E938-457D-BB91-89990D3D2810}" name="Table4913416" displayName="Table4913416" ref="I3:L8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BCD2CAA6-E938-457D-BB91-89990D3D2810}" name="Table4913416" displayName="Table4913416" ref="I3:L8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C991C267-3048-4225-B828-12E25D3E5025}" name="S/N" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{762A4A20-DDB2-474A-8744-7CECF83980B1}" name="Detection Count" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{08F95622-5A81-4212-AE47-92A0246F77EC}" name="Sample Size" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{52BB0AE4-B04C-4A77-962C-287EC8E5F665}" name="Accuracy" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{C991C267-3048-4225-B828-12E25D3E5025}" name="S/N" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{762A4A20-DDB2-474A-8744-7CECF83980B1}" name="Detection Count" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{08F95622-5A81-4212-AE47-92A0246F77EC}" name="Sample Size" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{52BB0AE4-B04C-4A77-962C-287EC8E5F665}" name="Accuracy" dataDxfId="54">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -949,13 +1065,13 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CB6C8DE4-CA53-4725-B7F8-AA492457AAE7}" name="Table461014717" displayName="Table461014717" ref="I13:L18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CB6C8DE4-CA53-4725-B7F8-AA492457AAE7}" name="Table461014717" displayName="Table461014717" ref="I13:L18" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9C4BC6FC-1B17-4A97-96D3-43004D220CAE}" name="S/N" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{15BE8F3E-E6BD-4F8A-A09A-BC176454914E}" name="Detection Count" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{A567ED6E-D3B6-4394-AF09-84C5732DC7B7}" name="Sample Size" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{5C74BD57-2650-4F27-A620-D6FE482814D1}" name="Accuracy" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{9C4BC6FC-1B17-4A97-96D3-43004D220CAE}" name="S/N" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{15BE8F3E-E6BD-4F8A-A09A-BC176454914E}" name="Detection Count" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{A567ED6E-D3B6-4394-AF09-84C5732DC7B7}" name="Sample Size" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{5C74BD57-2650-4F27-A620-D6FE482814D1}" name="Accuracy" dataDxfId="48">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -964,13 +1080,13 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{32A616EB-A77D-4F38-AEF8-2444FD4EF958}" name="Table4112818" displayName="Table4112818" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{32A616EB-A77D-4F38-AEF8-2444FD4EF958}" name="Table4112818" displayName="Table4112818" ref="D3:G8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2465D8E4-C5BF-4E81-AAEA-6B1E212E7BBD}" name="S/N" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{F0DD74ED-14AB-4A12-8DC6-7E49A5ACD8AC}" name="Detection Count" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{0681E460-8849-486E-8A3F-22055197C330}" name="Sample Size" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{6457E6E5-B2B0-4B8E-B3FB-47649ACD14D0}" name="Accuracy" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{2465D8E4-C5BF-4E81-AAEA-6B1E212E7BBD}" name="S/N" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{F0DD74ED-14AB-4A12-8DC6-7E49A5ACD8AC}" name="Detection Count" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{0681E460-8849-486E-8A3F-22055197C330}" name="Sample Size" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{6457E6E5-B2B0-4B8E-B3FB-47649ACD14D0}" name="Accuracy" dataDxfId="42">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -979,13 +1095,13 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{9CC61B1E-103F-4412-872D-2E234673F946}" name="Table461231519" displayName="Table461231519" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{9CC61B1E-103F-4412-872D-2E234673F946}" name="Table461231519" displayName="Table461231519" ref="D13:G18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F38C2E0-46F3-41C3-A5E6-EEEE64A2589F}" name="S/N" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{35F01D39-81DD-4978-AF87-26C70E04D654}" name="Detection Count" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{4744942B-C705-4E3F-A247-958A2EB2E913}" name="Sample Size" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{BBE1D400-C4DA-4403-BE90-442D8886004B}" name="Accuracy" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{9F38C2E0-46F3-41C3-A5E6-EEEE64A2589F}" name="S/N" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{35F01D39-81DD-4978-AF87-26C70E04D654}" name="Detection Count" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{4744942B-C705-4E3F-A247-958A2EB2E913}" name="Sample Size" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{BBE1D400-C4DA-4403-BE90-442D8886004B}" name="Accuracy" dataDxfId="36">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -994,13 +1110,13 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{589BC326-89DF-42FE-ADBB-E4FF113CEBDB}" name="Table491341620" displayName="Table491341620" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{589BC326-89DF-42FE-ADBB-E4FF113CEBDB}" name="Table491341620" displayName="Table491341620" ref="I3:L8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CCE9E2BE-0E17-41BE-967B-EE16AA992DDB}" name="S/N" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A7484308-39BA-4A28-9275-04DDFE2DFFEB}" name="Detection Count" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{2C4DCCF1-C4C2-4E4E-8BAF-B54EC7908178}" name="Sample Size" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{22839C3C-360C-4234-AFB5-FBBD81DFB55B}" name="Accuracy" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{CCE9E2BE-0E17-41BE-967B-EE16AA992DDB}" name="S/N" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{A7484308-39BA-4A28-9275-04DDFE2DFFEB}" name="Detection Count" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{2C4DCCF1-C4C2-4E4E-8BAF-B54EC7908178}" name="Sample Size" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{22839C3C-360C-4234-AFB5-FBBD81DFB55B}" name="Accuracy" dataDxfId="30">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1009,13 +1125,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="108">
+    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="132">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1024,13 +1140,73 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{6A0B21C2-72D0-4357-9836-2DED7539C21E}" name="Table46101471721" displayName="Table46101471721" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{6A0B21C2-72D0-4357-9836-2DED7539C21E}" name="Table46101471721" displayName="Table46101471721" ref="I13:L18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3258CFBC-6680-43C6-9D44-B8C132BDFF7E}" name="S/N" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{0C464FE1-A4AA-4ED8-8F75-83194D25D87B}" name="Detection Count" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{1977B50C-B9C1-44F2-BFF0-2D4C47585C51}" name="Sample Size" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{BA3CF17C-3E2E-4212-BDE3-20DA51952E02}" name="Accuracy" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{3258CFBC-6680-43C6-9D44-B8C132BDFF7E}" name="S/N" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{0C464FE1-A4AA-4ED8-8F75-83194D25D87B}" name="Detection Count" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{1977B50C-B9C1-44F2-BFF0-2D4C47585C51}" name="Sample Size" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{BA3CF17C-3E2E-4212-BDE3-20DA51952E02}" name="Accuracy" dataDxfId="24">
+      <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E682A1B8-92BF-48ED-8FA4-AF53F10103DE}" name="Table411281822" displayName="Table411281822" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{76656F77-3F63-4240-B7F2-57F941E82131}" name="S/N" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{042503D5-2728-4E0D-9F4E-7A2343CAF1A0}" name="Detection Count" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{3DBAB740-111F-4837-ABB6-1CE9A958B0E1}" name="Sample Size" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{44D1E94B-31CF-43FD-B07D-A021A7C3F17A}" name="Accuracy" dataDxfId="18">
+      <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{1E70F1A4-7B7F-44D6-A681-2DA8EF1E461E}" name="Table46123151923" displayName="Table46123151923" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{06E4C541-F18A-4436-ADA3-6128B41B1B9B}" name="S/N" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{524E748D-EAF2-4BF1-84E0-DAD83ACBC9CF}" name="Detection Count" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{D54A76B4-DB4B-4C99-AE5C-21FE05724C64}" name="Sample Size" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{F9C1B057-7F32-4879-BD1F-F5FA9C20ED5A}" name="Accuracy" dataDxfId="12">
+      <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{9C8629C9-BC78-4832-8138-7268A130A808}" name="Table49134162024" displayName="Table49134162024" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{216B3317-3137-45F8-963B-A74D575C7572}" name="S/N" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3E88BB9E-3C31-4E5E-B6BB-C99CA8E9F670}" name="Detection Count" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{33C2960E-2F38-4BF5-8424-AF88612B0E8D}" name="Sample Size" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{B9F5A5BF-ECFE-419C-B6BA-EE01F39F8ADD}" name="Accuracy" dataDxfId="6">
+      <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{379573D6-F606-4A4E-8F52-6C9D34B697BE}" name="Table4610147172125" displayName="Table4610147172125" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3DAC8C4E-FF84-42EF-9F60-988E00A40907}" name="S/N" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{C8D3EC17-3BE7-41FB-A79E-3C12FDCA7744}" name="Detection Count" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5633271A-EB23-40A1-AD8E-8678B5C9C3E7}" name="Sample Size" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6EAC7DA7-A60D-4A63-B6B6-F0F2B7E12B6A}" name="Accuracy" dataDxfId="0">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1039,13 +1215,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="102">
+    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="126">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1054,13 +1230,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="96">
+    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="120">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1069,13 +1245,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="90">
+    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="114">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1084,13 +1260,13 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="84">
+    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="108">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1099,13 +1275,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="102">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1114,13 +1290,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="96">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1129,13 +1305,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8836F220-A1C5-4260-B70B-3506874B3BA5}" name="Table4112" displayName="Table4112" ref="D3:G8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8836F220-A1C5-4260-B70B-3506874B3BA5}" name="Table4112" displayName="Table4112" ref="D3:G8" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B75D1CA6-6206-4228-BDCB-E56D23E710CF}" name="S/N" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{E0B715E6-3A0A-4312-B101-82F14F11CFBF}" name="Detection Count" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{72DD18F7-2B09-4F23-ADF4-C0C79EC302A9}" name="Sample Size" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{C140A7CC-F574-4E1F-8F2C-BD831A012684}" name="Accuracy" dataDxfId="66">
+    <tableColumn id="1" xr3:uid="{B75D1CA6-6206-4228-BDCB-E56D23E710CF}" name="S/N" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{E0B715E6-3A0A-4312-B101-82F14F11CFBF}" name="Detection Count" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{72DD18F7-2B09-4F23-ADF4-C0C79EC302A9}" name="Sample Size" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{C140A7CC-F574-4E1F-8F2C-BD831A012684}" name="Accuracy" dataDxfId="90">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3620,7 +3796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACAC222-742D-4DC0-B4CC-329DB85D9DEF}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -4162,4 +4338,564 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BFFB98-AD36-4576-AFC6-CF91E174B321}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>694</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>425</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2">
+        <v>332</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>222</v>
+      </c>
+      <c r="F4" s="10">
+        <v>222</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G8" si="0">(E4/F4)*100</f>
+        <v>100</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>296</v>
+      </c>
+      <c r="K4" s="10">
+        <v>299</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ref="L4:L8" si="1">(J4/K4)*100</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>79</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>222</v>
+      </c>
+      <c r="F5" s="10">
+        <v>222</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>296</v>
+      </c>
+      <c r="K5" s="10">
+        <v>299</v>
+      </c>
+      <c r="L5" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2">
+        <v>182</v>
+      </c>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10">
+        <v>222</v>
+      </c>
+      <c r="F6" s="10">
+        <v>222</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" s="10">
+        <v>296</v>
+      </c>
+      <c r="K6" s="10">
+        <v>299</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2">
+        <v>88</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10">
+        <v>222</v>
+      </c>
+      <c r="F7" s="10">
+        <v>222</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10">
+        <v>296</v>
+      </c>
+      <c r="K7" s="10">
+        <v>299</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUM(B2:B7)</f>
+        <v>1800</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>222</v>
+      </c>
+      <c r="F8" s="10">
+        <v>222</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+      <c r="J8" s="10">
+        <v>296</v>
+      </c>
+      <c r="K8" s="10">
+        <v>299</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8">
+        <f>AVERAGE(G4:G8)</f>
+        <v>100</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="8">
+        <f>AVERAGE(L4:L8)</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3">
+        <v>81</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3">
+        <v>56</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>46</v>
+      </c>
+      <c r="F14" s="10">
+        <v>56</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" ref="G14:G18" si="2">(E14/F14)*100</f>
+        <v>82.142857142857139</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
+        <v>32</v>
+      </c>
+      <c r="K14" s="10">
+        <v>299</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" ref="L14:L18" si="3">(J14/K14)*100</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>44</v>
+      </c>
+      <c r="F15" s="10">
+        <v>56</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="2"/>
+        <v>78.571428571428569</v>
+      </c>
+      <c r="I15" s="10">
+        <v>2</v>
+      </c>
+      <c r="J15" s="10">
+        <v>32</v>
+      </c>
+      <c r="K15" s="10">
+        <v>299</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUM(B11:B14)</f>
+        <v>182</v>
+      </c>
+      <c r="D16" s="10">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>42</v>
+      </c>
+      <c r="F16" s="10">
+        <v>56</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="I16" s="10">
+        <v>3</v>
+      </c>
+      <c r="J16" s="10">
+        <v>32</v>
+      </c>
+      <c r="K16" s="10">
+        <v>299</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="10">
+        <v>4</v>
+      </c>
+      <c r="E17" s="10">
+        <v>44</v>
+      </c>
+      <c r="F17" s="10">
+        <v>56</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="2"/>
+        <v>78.571428571428569</v>
+      </c>
+      <c r="I17" s="10">
+        <v>4</v>
+      </c>
+      <c r="J17" s="10">
+        <v>32</v>
+      </c>
+      <c r="K17" s="10">
+        <v>299</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B8+B16</f>
+        <v>1982</v>
+      </c>
+      <c r="D18" s="10">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>47</v>
+      </c>
+      <c r="F18" s="10">
+        <v>56</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="2"/>
+        <v>83.928571428571431</v>
+      </c>
+      <c r="I18" s="10">
+        <v>5</v>
+      </c>
+      <c r="J18" s="10">
+        <v>32</v>
+      </c>
+      <c r="K18" s="10">
+        <v>299</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="8">
+        <f>AVERAGE(G14:G18)</f>
+        <v>79.642857142857139</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="8">
+        <f>AVERAGE(L14:L18)</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13">
+        <f>AVERAGE(G10+G20)/2</f>
+        <v>89.821428571428569</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
serialized model v8, overall 93%, phishing 87%
</commit_message>
<xml_diff>
--- a/preprocessing/Model_Stats.xlsx
+++ b/preprocessing/Model_Stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon\Desktop\project-piscator\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E052E0-AAD0-4969-9DED-093723B42DF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663B08E3-2369-4EEA-99F8-212055B2D2A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
+    <workbookView xWindow="32820" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{96F4E3D8-3F5E-4126-898D-9C5F89A5C28C}"/>
   </bookViews>
   <sheets>
     <sheet name="V2" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="V5" sheetId="4" r:id="rId4"/>
     <sheet name="V6" sheetId="5" r:id="rId5"/>
     <sheet name="V7" sheetId="6" r:id="rId6"/>
+    <sheet name="V8" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="54">
   <si>
     <t>Jonathan_Mailbox</t>
   </si>
@@ -193,6 +194,16 @@
   <si>
     <t>Added about 40 mote items to train and increased phishing sample size. Model sits at about 79.6% right now, conclusion: requires more phishing emails</t>
   </si>
+  <si>
+    <t>ModernPhish4</t>
+  </si>
+  <si>
+    <t>dsv8.csv</t>
+  </si>
+  <si>
+    <t>Added about additional 36 phishing emails, 49/56 using ModernPhish3 to test. Overall at 93.2% and phish at 86.8%. 
+If the test set is added in to the dataset then the detection results are like 96% but that's kind of playing cheat</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +351,107 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="144">
+  <dxfs count="168">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -960,13 +1071,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F482A52D-BA7C-4E45-A2C5-7336D7E4750C}" name="Table4" displayName="Table4" ref="D3:G8" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="138">
+    <tableColumn id="1" xr3:uid="{C2E9D64F-51EC-4E67-A51C-F48A2432CF93}" name="S/N" dataDxfId="165"/>
+    <tableColumn id="2" xr3:uid="{CD28229E-530F-4DB0-A6C5-7BB5F4EC1DB3}" name="Detection Count" dataDxfId="164"/>
+    <tableColumn id="3" xr3:uid="{239F8F4B-5ED1-45A4-9AC7-42A8725D2C64}" name="Sample Size" dataDxfId="163"/>
+    <tableColumn id="4" xr3:uid="{4BC37E26-77BF-4D4D-8897-79CA92DB118A}" name="Accuracy" dataDxfId="162">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -975,13 +1086,13 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A3F97E-A535-4D7B-8BA9-370DCCBB0340}" name="Table46123" displayName="Table46123" ref="D13:G18" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A3F97E-A535-4D7B-8BA9-370DCCBB0340}" name="Table46123" displayName="Table46123" ref="D13:G18" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{275D5550-6ADB-43C4-BF7E-D2168244788F}" name="S/N" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{AD3A6138-B32C-4A9C-9861-0910BA8C7CF0}" name="Detection Count" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{53AB10D9-475E-498A-A010-18523684D9F0}" name="Sample Size" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{CCFFD2CF-6724-4423-818F-6CFEEFBF3A0E}" name="Accuracy" dataDxfId="84">
+    <tableColumn id="1" xr3:uid="{275D5550-6ADB-43C4-BF7E-D2168244788F}" name="S/N" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{AD3A6138-B32C-4A9C-9861-0910BA8C7CF0}" name="Detection Count" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{53AB10D9-475E-498A-A010-18523684D9F0}" name="Sample Size" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{CCFFD2CF-6724-4423-818F-6CFEEFBF3A0E}" name="Accuracy" dataDxfId="108">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -990,13 +1101,13 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B875B3D-C2EE-4CFF-BC4C-4BF1588E5042}" name="Table49134" displayName="Table49134" ref="I3:L8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5B875B3D-C2EE-4CFF-BC4C-4BF1588E5042}" name="Table49134" displayName="Table49134" ref="I3:L8" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E920ABA6-44F5-4C28-8A5E-0C0A6482E954}" name="S/N" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{0C7661B2-A4AD-4B35-8F73-6ED9583A18F9}" name="Detection Count" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{77DE6E9C-DB96-403B-9A7A-3CD37F43427E}" name="Sample Size" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{81917785-C766-46C0-A868-C83148F4C68F}" name="Accuracy" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{E920ABA6-44F5-4C28-8A5E-0C0A6482E954}" name="S/N" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{0C7661B2-A4AD-4B35-8F73-6ED9583A18F9}" name="Detection Count" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{77DE6E9C-DB96-403B-9A7A-3CD37F43427E}" name="Sample Size" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{81917785-C766-46C0-A868-C83148F4C68F}" name="Accuracy" dataDxfId="102">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1005,13 +1116,13 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2D337A66-8B74-438F-A66D-6DAE14683A0E}" name="Table4610147" displayName="Table4610147" ref="I13:L18" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2D337A66-8B74-438F-A66D-6DAE14683A0E}" name="Table4610147" displayName="Table4610147" ref="I13:L18" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E34AB060-FD1F-4F17-B6E3-FCB710023011}" name="S/N" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{7E19895C-182A-4984-AA78-7637705A8A27}" name="Detection Count" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{6D3C562D-AD07-4C05-820F-DBF3059539B1}" name="Sample Size" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{A053C10B-B044-4B72-912A-420CCD660884}" name="Accuracy" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{E34AB060-FD1F-4F17-B6E3-FCB710023011}" name="S/N" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{7E19895C-182A-4984-AA78-7637705A8A27}" name="Detection Count" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{6D3C562D-AD07-4C05-820F-DBF3059539B1}" name="Sample Size" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{A053C10B-B044-4B72-912A-420CCD660884}" name="Accuracy" dataDxfId="96">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1020,13 +1131,13 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15DF06F2-BFC5-400B-8F8E-C4A82BD5CA00}" name="Table41128" displayName="Table41128" ref="D3:G8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15DF06F2-BFC5-400B-8F8E-C4A82BD5CA00}" name="Table41128" displayName="Table41128" ref="D3:G8" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C753AC17-EEBF-4341-A85D-76065FABCBE7}" name="S/N" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{245102FA-69F1-4066-AF28-CCDAAA350CB3}" name="Detection Count" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{92689FC9-DDA3-4F25-8EFE-6CC23F93898B}" name="Sample Size" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{85C2FEF5-4AE8-4949-8ED0-C79CFBE661FB}" name="Accuracy" dataDxfId="66">
+    <tableColumn id="1" xr3:uid="{C753AC17-EEBF-4341-A85D-76065FABCBE7}" name="S/N" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{245102FA-69F1-4066-AF28-CCDAAA350CB3}" name="Detection Count" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{92689FC9-DDA3-4F25-8EFE-6CC23F93898B}" name="Sample Size" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{85C2FEF5-4AE8-4949-8ED0-C79CFBE661FB}" name="Accuracy" dataDxfId="90">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1035,13 +1146,13 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B5E58A1E-73FE-4AB3-B879-E930B517F804}" name="Table4612315" displayName="Table4612315" ref="D13:G18" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{B5E58A1E-73FE-4AB3-B879-E930B517F804}" name="Table4612315" displayName="Table4612315" ref="D13:G18" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{61A9D479-03E6-4200-94BF-A8DDEA70FEBF}" name="S/N" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{6050BD2E-D7F1-4053-A601-F41A8D89209F}" name="Detection Count" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{DD2DA752-841B-4E27-9369-82F77478078E}" name="Sample Size" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{64DD8FB3-6B62-43F6-89C0-49A140C3CF49}" name="Accuracy" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{61A9D479-03E6-4200-94BF-A8DDEA70FEBF}" name="S/N" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{6050BD2E-D7F1-4053-A601-F41A8D89209F}" name="Detection Count" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{DD2DA752-841B-4E27-9369-82F77478078E}" name="Sample Size" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{64DD8FB3-6B62-43F6-89C0-49A140C3CF49}" name="Accuracy" dataDxfId="84">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1050,13 +1161,13 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BCD2CAA6-E938-457D-BB91-89990D3D2810}" name="Table4913416" displayName="Table4913416" ref="I3:L8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BCD2CAA6-E938-457D-BB91-89990D3D2810}" name="Table4913416" displayName="Table4913416" ref="I3:L8" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C991C267-3048-4225-B828-12E25D3E5025}" name="S/N" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{762A4A20-DDB2-474A-8744-7CECF83980B1}" name="Detection Count" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{08F95622-5A81-4212-AE47-92A0246F77EC}" name="Sample Size" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{52BB0AE4-B04C-4A77-962C-287EC8E5F665}" name="Accuracy" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{C991C267-3048-4225-B828-12E25D3E5025}" name="S/N" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{762A4A20-DDB2-474A-8744-7CECF83980B1}" name="Detection Count" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{08F95622-5A81-4212-AE47-92A0246F77EC}" name="Sample Size" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{52BB0AE4-B04C-4A77-962C-287EC8E5F665}" name="Accuracy" dataDxfId="78">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1065,13 +1176,13 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CB6C8DE4-CA53-4725-B7F8-AA492457AAE7}" name="Table461014717" displayName="Table461014717" ref="I13:L18" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CB6C8DE4-CA53-4725-B7F8-AA492457AAE7}" name="Table461014717" displayName="Table461014717" ref="I13:L18" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9C4BC6FC-1B17-4A97-96D3-43004D220CAE}" name="S/N" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{15BE8F3E-E6BD-4F8A-A09A-BC176454914E}" name="Detection Count" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{A567ED6E-D3B6-4394-AF09-84C5732DC7B7}" name="Sample Size" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{5C74BD57-2650-4F27-A620-D6FE482814D1}" name="Accuracy" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{9C4BC6FC-1B17-4A97-96D3-43004D220CAE}" name="S/N" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{15BE8F3E-E6BD-4F8A-A09A-BC176454914E}" name="Detection Count" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{A567ED6E-D3B6-4394-AF09-84C5732DC7B7}" name="Sample Size" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{5C74BD57-2650-4F27-A620-D6FE482814D1}" name="Accuracy" dataDxfId="72">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1080,13 +1191,13 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{32A616EB-A77D-4F38-AEF8-2444FD4EF958}" name="Table4112818" displayName="Table4112818" ref="D3:G8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{32A616EB-A77D-4F38-AEF8-2444FD4EF958}" name="Table4112818" displayName="Table4112818" ref="D3:G8" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2465D8E4-C5BF-4E81-AAEA-6B1E212E7BBD}" name="S/N" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{F0DD74ED-14AB-4A12-8DC6-7E49A5ACD8AC}" name="Detection Count" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{0681E460-8849-486E-8A3F-22055197C330}" name="Sample Size" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{6457E6E5-B2B0-4B8E-B3FB-47649ACD14D0}" name="Accuracy" dataDxfId="42">
+    <tableColumn id="1" xr3:uid="{2465D8E4-C5BF-4E81-AAEA-6B1E212E7BBD}" name="S/N" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{F0DD74ED-14AB-4A12-8DC6-7E49A5ACD8AC}" name="Detection Count" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{0681E460-8849-486E-8A3F-22055197C330}" name="Sample Size" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{6457E6E5-B2B0-4B8E-B3FB-47649ACD14D0}" name="Accuracy" dataDxfId="66">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1095,13 +1206,13 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{9CC61B1E-103F-4412-872D-2E234673F946}" name="Table461231519" displayName="Table461231519" ref="D13:G18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{9CC61B1E-103F-4412-872D-2E234673F946}" name="Table461231519" displayName="Table461231519" ref="D13:G18" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F38C2E0-46F3-41C3-A5E6-EEEE64A2589F}" name="S/N" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{35F01D39-81DD-4978-AF87-26C70E04D654}" name="Detection Count" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{4744942B-C705-4E3F-A247-958A2EB2E913}" name="Sample Size" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{BBE1D400-C4DA-4403-BE90-442D8886004B}" name="Accuracy" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{9F38C2E0-46F3-41C3-A5E6-EEEE64A2589F}" name="S/N" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{35F01D39-81DD-4978-AF87-26C70E04D654}" name="Detection Count" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{4744942B-C705-4E3F-A247-958A2EB2E913}" name="Sample Size" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{BBE1D400-C4DA-4403-BE90-442D8886004B}" name="Accuracy" dataDxfId="60">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1110,13 +1221,13 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{589BC326-89DF-42FE-ADBB-E4FF113CEBDB}" name="Table491341620" displayName="Table491341620" ref="I3:L8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{589BC326-89DF-42FE-ADBB-E4FF113CEBDB}" name="Table491341620" displayName="Table491341620" ref="I3:L8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CCE9E2BE-0E17-41BE-967B-EE16AA992DDB}" name="S/N" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{A7484308-39BA-4A28-9275-04DDFE2DFFEB}" name="Detection Count" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{2C4DCCF1-C4C2-4E4E-8BAF-B54EC7908178}" name="Sample Size" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{22839C3C-360C-4234-AFB5-FBBD81DFB55B}" name="Accuracy" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{CCE9E2BE-0E17-41BE-967B-EE16AA992DDB}" name="S/N" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{A7484308-39BA-4A28-9275-04DDFE2DFFEB}" name="Detection Count" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{2C4DCCF1-C4C2-4E4E-8BAF-B54EC7908178}" name="Sample Size" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{22839C3C-360C-4234-AFB5-FBBD81DFB55B}" name="Accuracy" dataDxfId="54">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1125,13 +1236,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FA53D0D6-09B7-4E53-951C-1BC4BA64E6A9}" name="Table46" displayName="Table46" ref="D13:G18" totalsRowShown="0" headerRowDxfId="161" dataDxfId="160">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="134"/>
-    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="132">
+    <tableColumn id="1" xr3:uid="{57046574-AE69-4A16-AEFE-1BBDADE8D259}" name="S/N" dataDxfId="159"/>
+    <tableColumn id="2" xr3:uid="{8F88C883-E59A-4E69-8893-1152E6025CE8}" name="Detection Count" dataDxfId="158"/>
+    <tableColumn id="3" xr3:uid="{9020313D-2282-4852-8B4A-C1B95EE895A7}" name="Sample Size" dataDxfId="157"/>
+    <tableColumn id="4" xr3:uid="{B1DE2132-B81E-4BEE-9525-4E18279ABECB}" name="Accuracy" dataDxfId="156">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1140,13 +1251,13 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{6A0B21C2-72D0-4357-9836-2DED7539C21E}" name="Table46101471721" displayName="Table46101471721" ref="I13:L18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{6A0B21C2-72D0-4357-9836-2DED7539C21E}" name="Table46101471721" displayName="Table46101471721" ref="I13:L18" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3258CFBC-6680-43C6-9D44-B8C132BDFF7E}" name="S/N" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{0C464FE1-A4AA-4ED8-8F75-83194D25D87B}" name="Detection Count" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{1977B50C-B9C1-44F2-BFF0-2D4C47585C51}" name="Sample Size" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{BA3CF17C-3E2E-4212-BDE3-20DA51952E02}" name="Accuracy" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{3258CFBC-6680-43C6-9D44-B8C132BDFF7E}" name="S/N" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{0C464FE1-A4AA-4ED8-8F75-83194D25D87B}" name="Detection Count" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{1977B50C-B9C1-44F2-BFF0-2D4C47585C51}" name="Sample Size" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{BA3CF17C-3E2E-4212-BDE3-20DA51952E02}" name="Accuracy" dataDxfId="48">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1155,13 +1266,13 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E682A1B8-92BF-48ED-8FA4-AF53F10103DE}" name="Table411281822" displayName="Table411281822" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E682A1B8-92BF-48ED-8FA4-AF53F10103DE}" name="Table411281822" displayName="Table411281822" ref="D3:G8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{76656F77-3F63-4240-B7F2-57F941E82131}" name="S/N" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{042503D5-2728-4E0D-9F4E-7A2343CAF1A0}" name="Detection Count" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{3DBAB740-111F-4837-ABB6-1CE9A958B0E1}" name="Sample Size" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{44D1E94B-31CF-43FD-B07D-A021A7C3F17A}" name="Accuracy" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{76656F77-3F63-4240-B7F2-57F941E82131}" name="S/N" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{042503D5-2728-4E0D-9F4E-7A2343CAF1A0}" name="Detection Count" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{3DBAB740-111F-4837-ABB6-1CE9A958B0E1}" name="Sample Size" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{44D1E94B-31CF-43FD-B07D-A021A7C3F17A}" name="Accuracy" dataDxfId="42">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1170,13 +1281,13 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{1E70F1A4-7B7F-44D6-A681-2DA8EF1E461E}" name="Table46123151923" displayName="Table46123151923" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{1E70F1A4-7B7F-44D6-A681-2DA8EF1E461E}" name="Table46123151923" displayName="Table46123151923" ref="D13:G18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{06E4C541-F18A-4436-ADA3-6128B41B1B9B}" name="S/N" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{524E748D-EAF2-4BF1-84E0-DAD83ACBC9CF}" name="Detection Count" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{D54A76B4-DB4B-4C99-AE5C-21FE05724C64}" name="Sample Size" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{F9C1B057-7F32-4879-BD1F-F5FA9C20ED5A}" name="Accuracy" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{06E4C541-F18A-4436-ADA3-6128B41B1B9B}" name="S/N" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{524E748D-EAF2-4BF1-84E0-DAD83ACBC9CF}" name="Detection Count" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{D54A76B4-DB4B-4C99-AE5C-21FE05724C64}" name="Sample Size" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{F9C1B057-7F32-4879-BD1F-F5FA9C20ED5A}" name="Accuracy" dataDxfId="36">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1185,13 +1296,13 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{9C8629C9-BC78-4832-8138-7268A130A808}" name="Table49134162024" displayName="Table49134162024" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{9C8629C9-BC78-4832-8138-7268A130A808}" name="Table49134162024" displayName="Table49134162024" ref="I3:L8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{216B3317-3137-45F8-963B-A74D575C7572}" name="S/N" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{3E88BB9E-3C31-4E5E-B6BB-C99CA8E9F670}" name="Detection Count" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{33C2960E-2F38-4BF5-8424-AF88612B0E8D}" name="Sample Size" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{B9F5A5BF-ECFE-419C-B6BA-EE01F39F8ADD}" name="Accuracy" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{216B3317-3137-45F8-963B-A74D575C7572}" name="S/N" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{3E88BB9E-3C31-4E5E-B6BB-C99CA8E9F670}" name="Detection Count" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{33C2960E-2F38-4BF5-8424-AF88612B0E8D}" name="Sample Size" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{B9F5A5BF-ECFE-419C-B6BA-EE01F39F8ADD}" name="Accuracy" dataDxfId="30">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1200,13 +1311,73 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{379573D6-F606-4A4E-8F52-6C9D34B697BE}" name="Table4610147172125" displayName="Table4610147172125" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{379573D6-F606-4A4E-8F52-6C9D34B697BE}" name="Table4610147172125" displayName="Table4610147172125" ref="I13:L18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3DAC8C4E-FF84-42EF-9F60-988E00A40907}" name="S/N" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C8D3EC17-3BE7-41FB-A79E-3C12FDCA7744}" name="Detection Count" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{5633271A-EB23-40A1-AD8E-8678B5C9C3E7}" name="Sample Size" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{6EAC7DA7-A60D-4A63-B6B6-F0F2B7E12B6A}" name="Accuracy" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{3DAC8C4E-FF84-42EF-9F60-988E00A40907}" name="S/N" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{C8D3EC17-3BE7-41FB-A79E-3C12FDCA7744}" name="Detection Count" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{5633271A-EB23-40A1-AD8E-8678B5C9C3E7}" name="Sample Size" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{6EAC7DA7-A60D-4A63-B6B6-F0F2B7E12B6A}" name="Accuracy" dataDxfId="24">
+      <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{6CFEB867-7292-42D9-96FC-F1E46149661E}" name="Table41128182226" displayName="Table41128182226" ref="D3:G8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{AAF74251-CCC3-4C93-851C-C9FFF9027EED}" name="S/N" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{ED3FCCA0-0D17-4854-8578-A070835A8AA1}" name="Detection Count" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{3B4A61A6-6097-4791-98BD-61B4BCD398E2}" name="Sample Size" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{D279033F-9B2B-4065-A703-7311C794F914}" name="Accuracy" dataDxfId="18">
+      <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{B8DFE9EB-3E04-4953-A96C-34A240BD9176}" name="Table4612315192327" displayName="Table4612315192327" ref="D13:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FE5CA767-BF04-48A3-907C-C01AD399D772}" name="S/N" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1B0FDA70-248B-4D69-93F5-DDFC2CA51145}" name="Detection Count" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{449F2947-2429-46E3-A8EE-1F0343D2D7B8}" name="Sample Size" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{F9AAC848-6735-4B72-BED2-1F20E88E720B}" name="Accuracy" dataDxfId="12">
+      <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{9752B63F-B17B-4B6A-9619-24A116BCCDD3}" name="Table4913416202428" displayName="Table4913416202428" ref="I3:L8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{057B183E-2A2F-49B9-90E8-996EBA80399B}" name="S/N" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{E7973AC3-0400-4A49-BC84-470D211745B3}" name="Detection Count" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{73E8CEEC-1D20-41A5-AE2D-62882FEE3538}" name="Sample Size" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A1A3CD86-06F8-41E8-8D8E-96A37E2A364F}" name="Accuracy" dataDxfId="6">
+      <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{93D4AD38-3285-4454-9BE0-CD952E4DB1A2}" name="Table461014717212529" displayName="Table461014717212529" ref="I13:L18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B4847879-114B-4E60-9330-960BC1156108}" name="S/N" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{49F56172-53B2-4CD3-BA96-3028CB94D0B7}" name="Detection Count" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{55021D77-0320-4FE3-90D0-B4F052D4A964}" name="Sample Size" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{718C6904-4DC3-43BA-8317-BB231A922514}" name="Accuracy" dataDxfId="0">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1215,13 +1386,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{19ACEDF0-9288-4F0B-A7E8-F294251CC1B6}" name="Table49" displayName="Table49" ref="I3:L8" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="126">
+    <tableColumn id="1" xr3:uid="{ECDFB2A7-0F37-40DD-8DFC-F8D7E01FC52C}" name="S/N" dataDxfId="153"/>
+    <tableColumn id="2" xr3:uid="{013A58E9-6519-4A78-891F-AFB88B570A03}" name="Detection Count" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{C06B5641-FB89-4B0A-8000-995538E2ABA4}" name="Sample Size" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{757D148F-7916-4722-8308-0654D4FBA40A}" name="Accuracy" dataDxfId="150">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1230,13 +1401,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2376771A-EBDD-4008-8FB2-E0BE0CB8557D}" name="Table4610" displayName="Table4610" ref="I13:L18" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="120">
+    <tableColumn id="1" xr3:uid="{4B5E3E3B-362F-4267-828C-37512C450A50}" name="S/N" dataDxfId="147"/>
+    <tableColumn id="2" xr3:uid="{DDCF4B24-A327-4F23-BC57-F5BE50FBA07C}" name="Detection Count" dataDxfId="146"/>
+    <tableColumn id="3" xr3:uid="{17F1A410-59F1-4F19-B6A1-5DD90AD63BB0}" name="Sample Size" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{6826E5FA-8453-4CCB-8948-5F7BA63E070C}" name="Accuracy" dataDxfId="144">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1245,13 +1416,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EC07014E-6619-4C16-9664-C5427FE7802E}" name="Table411" displayName="Table411" ref="D3:G8" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="116"/>
-    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="114">
+    <tableColumn id="1" xr3:uid="{CE372C01-97F5-4077-98CB-EC0EFE0DBE79}" name="S/N" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{A2C4A0F1-B439-46C7-9877-AFF911A5B63A}" name="Detection Count" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{E3781A71-81B1-47F8-A7CD-8EC5545A9AAA}" name="Sample Size" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{C625D681-079D-4710-ADCF-98E8D12305D0}" name="Accuracy" dataDxfId="138">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1260,13 +1431,13 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{84850FC4-8FCF-4DDD-966A-1B2305A895C6}" name="Table4612" displayName="Table4612" ref="D13:G18" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
   <autoFilter ref="D13:G18" xr:uid="{7C1C5C4A-0633-4E95-B9F6-596D8846A469}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="108">
+    <tableColumn id="1" xr3:uid="{016C8EFE-BAC8-4478-8EA1-AB1CFC23A6DF}" name="S/N" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{C3FC55FD-739B-42E0-9549-E41AA1A3DB56}" name="Detection Count" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{F045AFE3-3E32-4E61-925B-CB13BAEDFEA3}" name="Sample Size" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{525F6BF9-037E-4BFF-8A51-FAB740F3EA4E}" name="Accuracy" dataDxfId="132">
       <calculatedColumnFormula>(E14/F14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1275,13 +1446,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D3577A01-A7DC-4A68-AE11-C5DE64850EF3}" name="Table4913" displayName="Table4913" ref="I3:L8" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
   <autoFilter ref="I3:L8" xr:uid="{A97E878C-96CA-4F6E-A5E0-B8DBAC528D86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="102">
+    <tableColumn id="1" xr3:uid="{AEAD603D-3D34-4A5F-82A4-7AFEE048278F}" name="S/N" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{C003332F-B1CD-4C00-951B-B7A884B23231}" name="Detection Count" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{78BCF4D9-9CC4-406B-AF86-B827AB6DF422}" name="Sample Size" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{1774E740-C43E-4E40-B1C7-9FCC7437BCD8}" name="Accuracy" dataDxfId="126">
       <calculatedColumnFormula>(J4/K4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1290,13 +1461,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7A289705-7896-494E-BB8D-AF6A27419594}" name="Table461014" displayName="Table461014" ref="I13:L18" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
   <autoFilter ref="I13:L18" xr:uid="{6578F40A-A8AE-4F7B-910D-2A8B15427FFA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="96">
+    <tableColumn id="1" xr3:uid="{3CC8EDC0-D921-4075-85EB-E1F8B9372262}" name="S/N" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{A639B1F3-E7FD-4775-8E50-442FE8DA5BA6}" name="Detection Count" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{E6B5163A-143C-489B-826A-EE4EF8313C37}" name="Sample Size" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{0F95D32D-CEAA-4734-86A9-968C63DF8ECC}" name="Accuracy" dataDxfId="120">
       <calculatedColumnFormula>(J14/K14)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1305,13 +1476,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8836F220-A1C5-4260-B70B-3506874B3BA5}" name="Table4112" displayName="Table4112" ref="D3:G8" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8836F220-A1C5-4260-B70B-3506874B3BA5}" name="Table4112" displayName="Table4112" ref="D3:G8" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="D3:G8" xr:uid="{D5B7493D-A0BD-41C2-902B-27DEECDC3668}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B75D1CA6-6206-4228-BDCB-E56D23E710CF}" name="S/N" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{E0B715E6-3A0A-4312-B101-82F14F11CFBF}" name="Detection Count" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{72DD18F7-2B09-4F23-ADF4-C0C79EC302A9}" name="Sample Size" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{C140A7CC-F574-4E1F-8F2C-BD831A012684}" name="Accuracy" dataDxfId="90">
+    <tableColumn id="1" xr3:uid="{B75D1CA6-6206-4228-BDCB-E56D23E710CF}" name="S/N" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{E0B715E6-3A0A-4312-B101-82F14F11CFBF}" name="Detection Count" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{72DD18F7-2B09-4F23-ADF4-C0C79EC302A9}" name="Sample Size" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{C140A7CC-F574-4E1F-8F2C-BD831A012684}" name="Accuracy" dataDxfId="114">
       <calculatedColumnFormula>(E4/F4)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4344,7 +4515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BFFB98-AD36-4576-AFC6-CF91E174B321}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -4898,4 +5069,568 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DF0871-2369-44A1-AD73-D7F43BCE618A}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>694</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>425</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2">
+        <v>332</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>237</v>
+      </c>
+      <c r="F4" s="10">
+        <v>238</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G8" si="0">(E4/F4)*100</f>
+        <v>99.579831932773118</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>296</v>
+      </c>
+      <c r="K4" s="10">
+        <v>299</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ref="L4:L8" si="1">(J4/K4)*100</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>79</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>237</v>
+      </c>
+      <c r="F5" s="10">
+        <v>238</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>99.579831932773118</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>296</v>
+      </c>
+      <c r="K5" s="10">
+        <v>299</v>
+      </c>
+      <c r="L5" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2">
+        <v>182</v>
+      </c>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="E6" s="10">
+        <v>237</v>
+      </c>
+      <c r="F6" s="10">
+        <v>238</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>99.579831932773118</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" s="10">
+        <v>296</v>
+      </c>
+      <c r="K6" s="10">
+        <v>299</v>
+      </c>
+      <c r="L6" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2">
+        <v>88</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" s="10">
+        <v>237</v>
+      </c>
+      <c r="F7" s="10">
+        <v>238</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>99.579831932773118</v>
+      </c>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10">
+        <v>296</v>
+      </c>
+      <c r="K7" s="10">
+        <v>299</v>
+      </c>
+      <c r="L7" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUM(B2:B7)</f>
+        <v>1800</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>237</v>
+      </c>
+      <c r="F8" s="10">
+        <v>238</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.579831932773118</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+      <c r="J8" s="10">
+        <v>296</v>
+      </c>
+      <c r="K8" s="10">
+        <v>299</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="1"/>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="F10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8">
+        <f>AVERAGE(G4:G8)</f>
+        <v>99.579831932773118</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="8">
+        <f>AVERAGE(L4:L8)</f>
+        <v>98.996655518394647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3">
+        <v>81</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3">
+        <v>56</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="3">
+        <v>36</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>49</v>
+      </c>
+      <c r="F14" s="10">
+        <v>56</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" ref="G14:G18" si="2">(E14/F14)*100</f>
+        <v>87.5</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
+        <v>32</v>
+      </c>
+      <c r="K14" s="10">
+        <v>299</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" ref="L14:L18" si="3">(J14/K14)*100</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="10">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>49</v>
+      </c>
+      <c r="F15" s="10">
+        <v>56</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="2"/>
+        <v>87.5</v>
+      </c>
+      <c r="I15" s="10">
+        <v>2</v>
+      </c>
+      <c r="J15" s="10">
+        <v>32</v>
+      </c>
+      <c r="K15" s="10">
+        <v>299</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUM(B11:B14)</f>
+        <v>218</v>
+      </c>
+      <c r="D16" s="10">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>49</v>
+      </c>
+      <c r="F16" s="10">
+        <v>56</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="2"/>
+        <v>87.5</v>
+      </c>
+      <c r="I16" s="10">
+        <v>3</v>
+      </c>
+      <c r="J16" s="10">
+        <v>32</v>
+      </c>
+      <c r="K16" s="10">
+        <v>299</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="10">
+        <v>4</v>
+      </c>
+      <c r="E17" s="10">
+        <v>47</v>
+      </c>
+      <c r="F17" s="10">
+        <v>56</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="2"/>
+        <v>83.928571428571431</v>
+      </c>
+      <c r="I17" s="10">
+        <v>4</v>
+      </c>
+      <c r="J17" s="10">
+        <v>32</v>
+      </c>
+      <c r="K17" s="10">
+        <v>299</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <f>B8+B16</f>
+        <v>2018</v>
+      </c>
+      <c r="D18" s="10">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>49</v>
+      </c>
+      <c r="F18" s="10">
+        <v>56</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="2"/>
+        <v>87.5</v>
+      </c>
+      <c r="I18" s="10">
+        <v>5</v>
+      </c>
+      <c r="J18" s="10">
+        <v>32</v>
+      </c>
+      <c r="K18" s="10">
+        <v>299</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="3"/>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="8">
+        <f>AVERAGE(G14:G18)</f>
+        <v>86.785714285714292</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="8">
+        <f>AVERAGE(L14:L18)</f>
+        <v>10.702341137123746</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13">
+        <f>AVERAGE(G10+G20)/2</f>
+        <v>93.182773109243698</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>